<commit_message>
working code for instruction list with Done
</commit_message>
<xml_diff>
--- a/class_labels.xlsx
+++ b/class_labels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004v8ph\Documents\Hackathon\Code\Object_Detection_YOLOv5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6FAF6F-E193-4D79-B20A-04C369E199C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AE1234-71FF-4B23-BAE5-27294891D682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Manifold Installed</t>
   </si>
@@ -49,6 +49,18 @@
   </si>
   <si>
     <t>Instruction Number</t>
+  </si>
+  <si>
+    <t>Empty Panel</t>
+  </si>
+  <si>
+    <t>Battery Not Installed</t>
+  </si>
+  <si>
+    <t>Screws Not Installed</t>
+  </si>
+  <si>
+    <t>M8 x 35 Screw</t>
   </si>
 </sst>
 </file>
@@ -84,9 +96,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +405,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,64 +417,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>-1</v>
+      </c>
+    </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>-1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes for Instruction and color with boxes for detection
</commit_message>
<xml_diff>
--- a/class_labels.xlsx
+++ b/class_labels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004v8ph\Documents\Hackathon\Code\Object_Detection_YOLOv5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AE1234-71FF-4B23-BAE5-27294891D682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4FA014-7B0D-409E-B898-8591F2B07166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -405,7 +405,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +429,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -437,7 +437,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -445,7 +445,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -453,7 +453,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -461,7 +461,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -469,7 +469,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Working code with next instruction styling and completed step styling
</commit_message>
<xml_diff>
--- a/class_labels.xlsx
+++ b/class_labels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004v8ph\Documents\Hackathon\Code\Object_Detection_YOLOv5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F4FA014-7B0D-409E-B898-8591F2B07166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39B6A20-C927-4DDA-A16E-A428E63FFF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Manifold Installed</t>
   </si>
@@ -61,6 +61,15 @@
   </si>
   <si>
     <t>M8 x 35 Screw</t>
+  </si>
+  <si>
+    <t>M_F Spacer Screw</t>
+  </si>
+  <si>
+    <t>1by4 x 1by2 Screw</t>
+  </si>
+  <si>
+    <t>1by4 x 1 Screw</t>
   </si>
 </sst>
 </file>
@@ -129,8 +138,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7A52BAAC-C930-41E3-9F74-B187DD785B55}" name="Table6" displayName="Table6" ref="A1:B11" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:B11" xr:uid="{7A52BAAC-C930-41E3-9F74-B187DD785B55}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{7A52BAAC-C930-41E3-9F74-B187DD785B55}" name="Table6" displayName="Table6" ref="A1:B14" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B14" xr:uid="{7A52BAAC-C930-41E3-9F74-B187DD785B55}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{5EF9D962-B78B-4DEE-9D82-11CE8F54DD14}" name="Class"/>
     <tableColumn id="2" xr3:uid="{B9640394-8281-46E2-8DBF-DDB757966319}" name="Instruction Number"/>
@@ -402,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,6 +423,7 @@
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -434,55 +444,55 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>-1</v>
@@ -490,10 +500,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -501,6 +511,30 @@
         <v>11</v>
       </c>
       <c r="B11">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
         <v>-1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working code with Mark as done
</commit_message>
<xml_diff>
--- a/class_labels.xlsx
+++ b/class_labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004v8ph\Documents\Hackathon\Code\Object_Detection_YOLOv5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39B6A20-C927-4DDA-A16E-A428E63FFF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97827CC-132B-419A-9F1B-660A7DA0C137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,7 +439,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -455,7 +455,7 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -471,7 +471,7 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -479,7 +479,7 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -487,7 +487,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -503,7 +503,7 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -519,7 +519,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>-1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -527,7 +527,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -535,7 +535,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
model execution with self training feature
</commit_message>
<xml_diff>
--- a/class_labels.xlsx
+++ b/class_labels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004v8ph\Documents\Hackathon\Code\Object_Detection_YOLOv5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97827CC-132B-419A-9F1B-660A7DA0C137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1A0154-C47D-41CD-8027-12A637024322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,7 +487,7 @@
         <v>4</v>
       </c>
       <c r="B8">
-        <v>-1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -527,7 +527,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>